<commit_message>
update and fix importing workflows
</commit_message>
<xml_diff>
--- a/InputData/PlatformOperation.xlsx
+++ b/InputData/PlatformOperation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PhD project\Products\Models\OffPlatfEner\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB78DAEA-4728-40CE-A681-3618D7E03F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D2E3C6-BFE4-45EB-B1E5-F27D8EA85817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12645" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="661" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="306">
   <si>
     <t>Specification document (open access)</t>
   </si>
@@ -1686,7 +1686,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1750,6 +1750,7 @@
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2138,7 +2139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7799,8 +7800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7922,6 +7923,9 @@
       <c r="C2" t="s">
         <v>162</v>
       </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
       <c r="I2" t="s">
         <v>184</v>
       </c>
@@ -7985,6 +7989,9 @@
       </c>
       <c r="C3" t="s">
         <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
       </c>
       <c r="I3" s="39" t="s">
         <v>184</v>
@@ -8174,7 +8181,7 @@
       <c r="C7" t="s">
         <v>167</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="39" t="s">
         <v>211</v>
       </c>
       <c r="F7" s="6">
@@ -8196,7 +8203,9 @@
       <c r="C8" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="D8" s="43"/>
+      <c r="D8" s="53" t="s">
+        <v>178</v>
+      </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -8210,6 +8219,9 @@
       </c>
       <c r="C9" t="s">
         <v>168</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>